<commit_message>
Se modifica la semana del 13 al 17 de febrero deacuerdo a los cambios que surguieron en el transcurso
</commit_message>
<xml_diff>
--- a/Calendario academico para info II.xlsx
+++ b/Calendario academico para info II.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UDEA\2023-1\Informatica-II\Teoria informatica II\Actividad02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCA7668-E10B-4F20-AFB8-575D54C1441D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8182C4-E6CC-400E-8B78-A9308D8EA2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{DA928043-3E6E-49B7-A1B1-1782E81C49CA}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="27240" windowHeight="15840" xr2:uid="{DA928043-3E6E-49B7-A1B1-1782E81C49CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feb 13 - 19" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="54">
   <si>
     <t>Lunes</t>
   </si>
@@ -169,10 +169,6 @@
   <si>
     <t>Clase Electiva Actividades Atleticas
 - Ciclismo</t>
-  </si>
-  <si>
-    <t>Lab Info II
-- Practica 1</t>
   </si>
   <si>
     <t>Lab Circuitos II
@@ -285,7 +281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -491,11 +487,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -518,122 +551,112 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -951,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59E58C9-727E-4EBE-9E69-903BB75FA16B}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,16 +986,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
@@ -1002,25 +1025,25 @@
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="13">
         <v>13</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="10">
         <v>14</v>
       </c>
-      <c r="D3" s="11">
-        <v>15</v>
-      </c>
-      <c r="E3" s="11">
+      <c r="D3" s="10">
+        <v>15</v>
+      </c>
+      <c r="E3" s="10">
         <v>16</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <v>17</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="10">
         <v>18</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="10">
         <v>19</v>
       </c>
     </row>
@@ -1028,47 +1051,47 @@
       <c r="A4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="30"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="22"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="32"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="18" t="s">
+      <c r="D6" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="34"/>
+      <c r="F6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="25"/>
       <c r="I6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1077,34 +1100,34 @@
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="13"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="37"/>
+      <c r="B8" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="39"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="24"/>
       <c r="I8" s="4" t="s">
         <v>14</v>
       </c>
@@ -1113,31 +1136,31 @@
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="13"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="14" t="s">
+      <c r="B10" s="23"/>
+      <c r="C10" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="12" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1145,52 +1168,54 @@
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="23"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="12"/>
+      <c r="B11" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="40"/>
+      <c r="D11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="11"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="43"/>
+      <c r="C12" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="37"/>
+      <c r="E12" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="46"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="39" t="s">
+      <c r="B13" s="43"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="34" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1198,31 +1223,29 @@
       <c r="A14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="39"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="40"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="24" t="s">
+      <c r="B15" s="43"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="40" t="s">
+      <c r="H15" s="33" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1230,15 +1253,15 @@
       <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="40"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="33"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -1247,67 +1270,75 @@
       <c r="B17" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="24" t="s">
+      <c r="C17" s="41"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="40"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="33"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="42"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="34"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="25"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="42"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="34"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="25"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="34"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="25"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="47"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="25">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="E17:E19"/>
     <mergeCell ref="H15:H17"/>
     <mergeCell ref="H13:H14"/>
     <mergeCell ref="G13:G14"/>
@@ -1318,22 +1349,11 @@
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E14:E15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="G15:G17"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="F11:F15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1357,16 +1377,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
@@ -1422,47 +1442,47 @@
       <c r="A4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="30"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="22"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="32"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="18" t="s">
+      <c r="B6" s="40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="18" t="s">
+      <c r="D6" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="34"/>
+      <c r="F6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="25"/>
       <c r="I6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1471,34 +1491,34 @@
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="13"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="37"/>
+      <c r="B8" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="39"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="24"/>
       <c r="I8" s="4" t="s">
         <v>14</v>
       </c>
@@ -1507,31 +1527,31 @@
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="13"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="17" t="s">
+      <c r="B10" s="23"/>
+      <c r="C10" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="48" t="s">
+      <c r="D10" s="14"/>
+      <c r="E10" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="14" t="s">
+      <c r="F10" s="14"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="12" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1539,52 +1559,52 @@
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="48"/>
-      <c r="F11" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="23"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="12"/>
+      <c r="B11" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="40"/>
+      <c r="D11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="11"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="43"/>
+      <c r="C12" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="37"/>
+      <c r="E12" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="35"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="39" t="s">
+      <c r="B13" s="43"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="34" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1592,31 +1612,31 @@
       <c r="A14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="39"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="40"/>
+      <c r="E14" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="24" t="s">
+      <c r="B15" s="43"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="40" t="s">
+      <c r="H15" s="33" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1624,15 +1644,15 @@
       <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="40"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="33"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -1641,76 +1661,72 @@
       <c r="B17" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="24" t="s">
+      <c r="C17" s="40"/>
+      <c r="D17" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="40"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="33"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="42"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="34"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="25"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="42"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="34"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="25"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="34"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="25"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="47"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E7"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
@@ -1722,12 +1738,16 @@
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D15"/>
     <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="C16:C18"/>
     <mergeCell ref="G13:G14"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1750,16 +1770,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
@@ -1786,8 +1806,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
-        <v>48</v>
+      <c r="A3" s="32" t="s">
+        <v>47</v>
       </c>
       <c r="B3" s="1">
         <v>27</v>
@@ -1815,47 +1835,47 @@
       <c r="A4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="30"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="22"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="32"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="18" t="s">
+      <c r="B6" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="18" t="s">
+      <c r="D6" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="34"/>
+      <c r="F6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="25"/>
       <c r="I6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1864,34 +1884,34 @@
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="13"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="37"/>
+      <c r="B8" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="39"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="24"/>
       <c r="I8" s="4" t="s">
         <v>14</v>
       </c>
@@ -1900,31 +1920,31 @@
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="13"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="48" t="s">
+      <c r="B10" s="23"/>
+      <c r="C10" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="14" t="s">
+      <c r="F10" s="14"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="12" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1932,52 +1952,52 @@
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="48"/>
-      <c r="F11" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="23"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="12"/>
+      <c r="B11" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="40"/>
+      <c r="D11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="11"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="43"/>
+      <c r="C12" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="37"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="39" t="s">
+      <c r="B13" s="43"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="34" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1985,31 +2005,31 @@
       <c r="A14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="39"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="40"/>
+      <c r="E14" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="24" t="s">
+      <c r="B15" s="43"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="40" t="s">
+      <c r="H15" s="33" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2017,15 +2037,15 @@
       <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="40"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="33"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -2034,74 +2054,74 @@
       <c r="B17" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="24" t="s">
+      <c r="C17" s="40"/>
+      <c r="D17" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="40"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="33"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="42"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="34"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="25"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="42"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="34"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="25"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="34"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="25"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="47"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E7"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
@@ -2113,14 +2133,14 @@
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D15"/>
     <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
     <mergeCell ref="G13:G14"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2131,7 +2151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A1E6B1-1672-4BD3-B740-6945467D3870}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -2143,16 +2163,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
@@ -2208,157 +2228,157 @@
       <c r="A4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="30"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="22"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="32"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="18" t="s">
+      <c r="B6" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="18" t="s">
+      <c r="D6" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="34"/>
+      <c r="F6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="25"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="49"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="34"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="25"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="37"/>
+      <c r="B8" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="39"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="24"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="37"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="24"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="48" t="s">
+      <c r="B10" s="23"/>
+      <c r="C10" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="38"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="48"/>
-      <c r="F11" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="23"/>
-      <c r="H11" s="38"/>
+      <c r="B11" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="40"/>
+      <c r="D11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="40"/>
+      <c r="F11" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="43"/>
+      <c r="C12" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="37"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="39" t="s">
+      <c r="B13" s="43"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="34" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2366,31 +2386,31 @@
       <c r="A14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="39"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="40"/>
+      <c r="E14" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="24" t="s">
+      <c r="B15" s="43"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="40" t="s">
+      <c r="H15" s="33" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2398,15 +2418,15 @@
       <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="40"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="33"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -2415,76 +2435,74 @@
       <c r="B17" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="24" t="s">
+      <c r="C17" s="40"/>
+      <c r="D17" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="40"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="33"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="42"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="34"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="25"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="42"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="34"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="25"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="34"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="25"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="45"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="47"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E7"/>
     <mergeCell ref="F7:F9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
@@ -2495,13 +2513,15 @@
     <mergeCell ref="F11:F15"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D15"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="D6:D9"/>
-    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="C16:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>